<commit_message>
Added correct dataset and updated analysis
</commit_message>
<xml_diff>
--- a/datasets/Oreos.xlsx
+++ b/datasets/Oreos.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10614"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anitaowens/Documents/GitHub/Forecasting-in-Python/datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5695C65-EA5F-264D-926D-49B8720FEAC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D007A5CE-89FD-EC4A-A44E-B06305CE4DFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8380" yWindow="500" windowWidth="28800" windowHeight="16120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="3" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterateDelta="1.0000000000000001E-5"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -378,7 +378,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A5"/>
+      <selection activeCell="C2" sqref="C2:C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -406,8 +406,7 @@
         <v>5</v>
       </c>
       <c r="C2">
-        <f ca="1">40+RANDBETWEEN(-10,10)+IF(B2=5,-10,IF(B2=6,20,0))</f>
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -418,8 +417,7 @@
         <v>6</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C13" ca="1" si="0">40+RANDBETWEEN(-10,10)+IF(B3=5,-10,IF(B3=6,20,0))</f>
-        <v>67</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -430,7 +428,6 @@
         <v>7</v>
       </c>
       <c r="C4">
-        <f t="shared" ca="1" si="0"/>
         <v>40</v>
       </c>
     </row>
@@ -442,8 +439,7 @@
         <v>5</v>
       </c>
       <c r="C5">
-        <f t="shared" ca="1" si="0"/>
-        <v>40</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -454,8 +450,7 @@
         <v>5</v>
       </c>
       <c r="C6">
-        <f t="shared" ca="1" si="0"/>
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -466,8 +461,7 @@
         <v>6</v>
       </c>
       <c r="C7">
-        <f t="shared" ca="1" si="0"/>
-        <v>55</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -478,8 +472,7 @@
         <v>6</v>
       </c>
       <c r="C8">
-        <f t="shared" ca="1" si="0"/>
-        <v>63</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -490,8 +483,7 @@
         <v>7</v>
       </c>
       <c r="C9">
-        <f t="shared" ca="1" si="0"/>
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -502,8 +494,7 @@
         <v>7</v>
       </c>
       <c r="C10">
-        <f t="shared" ca="1" si="0"/>
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -514,8 +505,7 @@
         <v>5</v>
       </c>
       <c r="C11">
-        <f t="shared" ca="1" si="0"/>
-        <v>30</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -526,8 +516,7 @@
         <v>6</v>
       </c>
       <c r="C12">
-        <f t="shared" ca="1" si="0"/>
-        <v>55</v>
+        <v>63</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -538,8 +527,7 @@
         <v>7</v>
       </c>
       <c r="C13">
-        <f t="shared" ca="1" si="0"/>
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -586,7 +574,7 @@
       </c>
       <c r="G7">
         <f ca="1">40+RANDBETWEEN(-10,10)+IF(F7=5,-10,IF(F7=6,20,0))</f>
-        <v>20</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="5:7" x14ac:dyDescent="0.2">
@@ -598,7 +586,7 @@
       </c>
       <c r="G8">
         <f t="shared" ref="G8:G18" ca="1" si="0">40+RANDBETWEEN(-10,10)+IF(F8=5,-10,IF(F8=6,20,0))</f>
-        <v>62</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="5:7" x14ac:dyDescent="0.2">
@@ -610,7 +598,7 @@
       </c>
       <c r="G9">
         <f t="shared" ca="1" si="0"/>
-        <v>36</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="5:7" x14ac:dyDescent="0.2">
@@ -622,7 +610,7 @@
       </c>
       <c r="G10">
         <f t="shared" ca="1" si="0"/>
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="5:7" x14ac:dyDescent="0.2">
@@ -634,7 +622,7 @@
       </c>
       <c r="G11">
         <f t="shared" ca="1" si="0"/>
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="5:7" x14ac:dyDescent="0.2">
@@ -646,7 +634,7 @@
       </c>
       <c r="G12">
         <f t="shared" ca="1" si="0"/>
-        <v>70</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="5:7" x14ac:dyDescent="0.2">
@@ -658,7 +646,7 @@
       </c>
       <c r="G13">
         <f t="shared" ca="1" si="0"/>
-        <v>63</v>
+        <v>70</v>
       </c>
     </row>
     <row r="14" spans="5:7" x14ac:dyDescent="0.2">
@@ -670,7 +658,7 @@
       </c>
       <c r="G14">
         <f t="shared" ca="1" si="0"/>
-        <v>37</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="5:7" x14ac:dyDescent="0.2">
@@ -682,7 +670,7 @@
       </c>
       <c r="G15">
         <f t="shared" ca="1" si="0"/>
-        <v>50</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="5:7" x14ac:dyDescent="0.2">
@@ -694,7 +682,7 @@
       </c>
       <c r="G16">
         <f t="shared" ca="1" si="0"/>
-        <v>32</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="5:7" x14ac:dyDescent="0.2">
@@ -706,7 +694,7 @@
       </c>
       <c r="G17">
         <f t="shared" ca="1" si="0"/>
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="18" spans="5:7" x14ac:dyDescent="0.2">
@@ -718,7 +706,7 @@
       </c>
       <c r="G18">
         <f t="shared" ca="1" si="0"/>
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>